<commit_message>
Fixed errors in NOAA site file to match Steve's comments
</commit_message>
<xml_diff>
--- a/NOAA/noaaSiteInformationUpdated.xlsx
+++ b/NOAA/noaaSiteInformationUpdated.xlsx
@@ -1,21 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/NOAA/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_0D99672CB05B5C388329DAD9A3DA230B9ECBE238" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{355C177A-53A2-4713-B2A4-EB2477150A8A}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="siteNameMapping"/>
-    <sheet r:id="rId2" sheetId="2" name="siteInformation"/>
+    <sheet name="siteNameMapping" sheetId="1" r:id="rId1"/>
+    <sheet name="siteInformation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="91">
   <si>
     <t>Station:</t>
   </si>
@@ -275,20 +294,25 @@
     <t>hope65</t>
   </si>
   <si>
-    <t>see coordinates list (in Muskegon Lake)</t>
-  </si>
-  <si>
     <t>temp</t>
   </si>
   <si>
     <t>x2</t>
+  </si>
+  <si>
+    <t>KV fixed coordinates to match other e sites, per Steve's comment</t>
+  </si>
+  <si>
+    <t>see coordinates list (in Muskegon Lake) - KV changed to KEEP==F per Steve comment</t>
+  </si>
+  <si>
+    <t>KV changed to KEEP=T because 8 is omega. Seems to have been a copy/paste error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -313,7 +337,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -343,16 +367,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -360,65 +384,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -429,10 +461,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -470,71 +502,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -562,7 +594,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -585,11 +617,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -598,13 +630,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -614,7 +646,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -623,7 +655,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -632,7 +664,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -640,10 +672,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -708,26 +740,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
@@ -750,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -761,17 +793,17 @@
         <v>27</v>
       </c>
       <c r="D2" s="6">
-        <v>43.18816667</v>
+        <v>43.188166670000001</v>
       </c>
       <c r="E2" s="6">
-        <v>-86.344</v>
+        <v>-86.343999999999994</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -782,17 +814,17 @@
         <v>29</v>
       </c>
       <c r="D3" s="6">
-        <v>43.18816667</v>
+        <v>43.188166670000001</v>
       </c>
       <c r="E3" s="6">
-        <v>-86.344</v>
+        <v>-86.343999999999994</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -803,17 +835,17 @@
         <v>30</v>
       </c>
       <c r="D4" s="6">
-        <v>43.18816667</v>
+        <v>43.188166670000001</v>
       </c>
       <c r="E4" s="6">
-        <v>-86.344</v>
+        <v>-86.343999999999994</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -824,17 +856,17 @@
         <v>31</v>
       </c>
       <c r="D5" s="6">
-        <v>43.18816667</v>
+        <v>43.188166670000001</v>
       </c>
       <c r="E5" s="6">
-        <v>-86.344</v>
+        <v>-86.343999999999994</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -845,17 +877,17 @@
         <v>32</v>
       </c>
       <c r="D6" s="6">
-        <v>43.20616667</v>
+        <v>43.206166670000002</v>
       </c>
       <c r="E6" s="6">
-        <v>-86.44966667</v>
+        <v>-86.449666669999999</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -866,17 +898,17 @@
         <v>33</v>
       </c>
       <c r="D7" s="6">
-        <v>43.20616667</v>
+        <v>43.206166670000002</v>
       </c>
       <c r="E7" s="6">
-        <v>-86.44966667</v>
+        <v>-86.449666669999999</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -887,17 +919,17 @@
         <v>34</v>
       </c>
       <c r="D8" s="6">
-        <v>43.20616667</v>
+        <v>43.206166670000002</v>
       </c>
       <c r="E8" s="6">
-        <v>-86.44966667</v>
+        <v>-86.449666669999999</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -908,17 +940,17 @@
         <v>35</v>
       </c>
       <c r="D9" s="6">
-        <v>43.20616667</v>
+        <v>43.206166670000002</v>
       </c>
       <c r="E9" s="6">
-        <v>-86.44966667</v>
+        <v>-86.449666669999999</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -929,17 +961,17 @@
         <v>36</v>
       </c>
       <c r="D10" s="6">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E10" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
@@ -950,17 +982,17 @@
         <v>37</v>
       </c>
       <c r="D11" s="6">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E11" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
@@ -971,17 +1003,17 @@
         <v>38</v>
       </c>
       <c r="D12" s="6">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E12" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -992,17 +1024,17 @@
         <v>39</v>
       </c>
       <c r="D13" s="6">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E13" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -1013,17 +1045,17 @@
         <v>40</v>
       </c>
       <c r="D14" s="6">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E14" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G14" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
@@ -1034,10 +1066,10 @@
         <v>41</v>
       </c>
       <c r="D15" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E15" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>42</v>
@@ -1046,7 +1078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>36</v>
       </c>
@@ -1057,10 +1089,10 @@
         <v>44</v>
       </c>
       <c r="D16" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E16" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>42</v>
@@ -1069,7 +1101,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>36</v>
       </c>
@@ -1080,10 +1112,10 @@
         <v>45</v>
       </c>
       <c r="D17" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E17" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>42</v>
@@ -1092,7 +1124,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
@@ -1103,10 +1135,10 @@
         <v>46</v>
       </c>
       <c r="D18" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E18" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>42</v>
@@ -1115,7 +1147,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>36</v>
       </c>
@@ -1126,10 +1158,10 @@
         <v>48</v>
       </c>
       <c r="D19" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E19" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>42</v>
@@ -1138,7 +1170,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
         <v>36</v>
       </c>
@@ -1149,10 +1181,10 @@
         <v>49</v>
       </c>
       <c r="D20" s="16">
-        <v>43.19983333</v>
+        <v>43.199833329999997</v>
       </c>
       <c r="E20" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>42</v>
@@ -1161,30 +1193,30 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="18">
         <v>110</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="16">
-        <v>43.19983333</v>
+      <c r="D21" s="19">
+        <v>43.199833329999997</v>
       </c>
       <c r="E21" s="6">
-        <v>-86.56983333</v>
+        <v>-86.569833329999994</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>51</v>
       </c>
@@ -1195,17 +1227,17 @@
         <v>51</v>
       </c>
       <c r="D22" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E22" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
@@ -1216,17 +1248,17 @@
         <v>52</v>
       </c>
       <c r="D23" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E23" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>51</v>
       </c>
@@ -1237,17 +1269,17 @@
         <v>53</v>
       </c>
       <c r="D24" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E24" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>51</v>
       </c>
@@ -1258,17 +1290,17 @@
         <v>54</v>
       </c>
       <c r="D25" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E25" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
@@ -1279,17 +1311,17 @@
         <v>55</v>
       </c>
       <c r="D26" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E26" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row r="27" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -1300,17 +1332,17 @@
         <v>56</v>
       </c>
       <c r="D27" s="6">
-        <v>43.01933333</v>
+        <v>43.019333330000002</v>
       </c>
       <c r="E27" s="6">
-        <v>-86.63183333</v>
+        <v>-86.631833330000006</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row r="28" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -1321,17 +1353,17 @@
         <v>57</v>
       </c>
       <c r="D28" s="6">
-        <v>43.0414</v>
+        <v>43.041400000000003</v>
       </c>
       <c r="E28" s="6">
-        <v>-86.3332</v>
+        <v>-86.333200000000005</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row r="29" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
@@ -1342,17 +1374,17 @@
         <v>58</v>
       </c>
       <c r="D29" s="6">
-        <v>43.07281667</v>
+        <v>43.072816670000002</v>
       </c>
       <c r="E29" s="6">
-        <v>-86.27886667</v>
+        <v>-86.278866669999999</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G29" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row r="30" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>58</v>
       </c>
@@ -1363,17 +1395,17 @@
         <v>59</v>
       </c>
       <c r="D30" s="6">
-        <v>43.07281667</v>
+        <v>43.072816670000002</v>
       </c>
       <c r="E30" s="6">
-        <v>-86.27886667</v>
+        <v>-86.278866669999999</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row r="31" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>60</v>
       </c>
@@ -1384,7 +1416,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="6">
-        <v>42.71033333</v>
+        <v>42.710333329999997</v>
       </c>
       <c r="E31" s="6">
         <v>-87.09483333</v>
@@ -1394,7 +1426,7 @@
       </c>
       <c r="G31" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row r="32" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
@@ -1405,17 +1437,17 @@
         <v>61</v>
       </c>
       <c r="D32" s="6">
-        <v>43.22016667</v>
+        <v>43.220166669999998</v>
       </c>
       <c r="E32" s="6">
-        <v>-86.35416667</v>
+        <v>-86.354166669999998</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G32" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row r="33" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>61</v>
       </c>
@@ -1426,17 +1458,17 @@
         <v>62</v>
       </c>
       <c r="D33" s="6">
-        <v>43.22016667</v>
+        <v>43.220166669999998</v>
       </c>
       <c r="E33" s="6">
-        <v>-86.35416667</v>
+        <v>-86.354166669999998</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>61</v>
       </c>
@@ -1447,17 +1479,17 @@
         <v>63</v>
       </c>
       <c r="D34" s="6">
-        <v>43.22016667</v>
+        <v>43.220166669999998</v>
       </c>
       <c r="E34" s="6">
-        <v>-86.35416667</v>
+        <v>-86.354166669999998</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G34" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row r="35" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>61</v>
       </c>
@@ -1468,17 +1500,17 @@
         <v>64</v>
       </c>
       <c r="D35" s="6">
-        <v>43.22016667</v>
+        <v>43.220166669999998</v>
       </c>
       <c r="E35" s="6">
-        <v>-86.35416667</v>
+        <v>-86.354166669999998</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G35" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row r="36" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>61</v>
       </c>
@@ -1489,17 +1521,17 @@
         <v>65</v>
       </c>
       <c r="D36" s="6">
-        <v>43.22016667</v>
+        <v>43.220166669999998</v>
       </c>
       <c r="E36" s="6">
-        <v>-86.35416667</v>
+        <v>-86.354166669999998</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G36" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>66</v>
       </c>
@@ -1513,14 +1545,14 @@
         <v>43.14233333</v>
       </c>
       <c r="E37" s="6">
-        <v>-86.29933333</v>
+        <v>-86.299333329999996</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>66</v>
       </c>
@@ -1534,14 +1566,14 @@
         <v>43.14233333</v>
       </c>
       <c r="E38" s="6">
-        <v>-86.29933333</v>
+        <v>-86.299333329999996</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G38" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>66</v>
       </c>
@@ -1555,14 +1587,14 @@
         <v>43.14233333</v>
       </c>
       <c r="E39" s="6">
-        <v>-86.29933333</v>
+        <v>-86.299333329999996</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G39" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>66</v>
       </c>
@@ -1576,14 +1608,14 @@
         <v>43.14233333</v>
       </c>
       <c r="E40" s="6">
-        <v>-86.29933333</v>
+        <v>-86.299333329999996</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G40" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>66</v>
       </c>
@@ -1597,14 +1629,14 @@
         <v>43.14233333</v>
       </c>
       <c r="E41" s="6">
-        <v>-86.29933333</v>
+        <v>-86.299333329999996</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G41" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row r="42" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>71</v>
       </c>
@@ -1615,17 +1647,19 @@
         <v>72</v>
       </c>
       <c r="D42" s="16">
-        <v>43.14233333</v>
+        <v>43.053666669999998</v>
       </c>
       <c r="E42" s="6">
-        <v>-86.29933333</v>
+        <v>-86.262833330000007</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+      <c r="G42" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>71</v>
       </c>
@@ -1636,17 +1670,17 @@
         <v>71</v>
       </c>
       <c r="D43" s="16">
-        <v>43.05366667</v>
+        <v>43.053666669999998</v>
       </c>
       <c r="E43" s="6">
-        <v>-86.26283333</v>
+        <v>-86.262833330000007</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G43" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>71</v>
       </c>
@@ -1657,17 +1691,17 @@
         <v>73</v>
       </c>
       <c r="D44" s="16">
-        <v>43.05366667</v>
+        <v>43.053666669999998</v>
       </c>
       <c r="E44" s="6">
-        <v>-86.26283333</v>
+        <v>-86.262833330000007</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row r="45" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>71</v>
       </c>
@@ -1678,17 +1712,17 @@
         <v>74</v>
       </c>
       <c r="D45" s="16">
-        <v>43.05366667</v>
+        <v>43.053666669999998</v>
       </c>
       <c r="E45" s="6">
-        <v>-86.26283333</v>
+        <v>-86.262833330000007</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G45" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>71</v>
       </c>
@@ -1699,17 +1733,17 @@
         <v>75</v>
       </c>
       <c r="D46" s="16">
-        <v>43.05366667</v>
+        <v>43.053666669999998</v>
       </c>
       <c r="E46" s="6">
-        <v>-86.26283333</v>
+        <v>-86.262833330000007</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>28</v>
       </c>
       <c r="G46" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row r="47" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="8"/>
       <c r="C47" s="4" t="s">
@@ -1724,7 +1758,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row r="48" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="8"/>
       <c r="C48" s="4" t="s">
@@ -1739,7 +1773,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row r="49" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>79</v>
       </c>
@@ -1753,7 +1787,7 @@
         <v>43.2</v>
       </c>
       <c r="E49" s="6">
-        <v>-86.37783333333333</v>
+        <v>-86.377833333333328</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>28</v>
@@ -1762,7 +1796,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row r="50" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>81</v>
       </c>
@@ -1773,10 +1807,10 @@
         <v>81</v>
       </c>
       <c r="D50" s="6">
-        <v>43.0598</v>
+        <v>43.059800000000003</v>
       </c>
       <c r="E50" s="6">
-        <v>-86.64833333333333</v>
+        <v>-86.648333333333326</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>28</v>
@@ -1785,7 +1819,7 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row r="51" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="8"/>
       <c r="C51" s="4" t="s">
@@ -1800,7 +1834,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row r="52" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="8"/>
       <c r="C52" s="4" t="s">
@@ -1815,7 +1849,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row r="53" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4"/>
       <c r="B53" s="8"/>
       <c r="C53" s="4" t="s">
@@ -1830,7 +1864,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row r="54" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>19</v>
       </c>
@@ -1841,23 +1875,23 @@
         <v>19</v>
       </c>
       <c r="D54" s="6">
-        <v>43.222166666666666</v>
+        <v>43.222166666666702</v>
       </c>
       <c r="E54" s="6">
-        <v>-86.28081666666667</v>
+        <v>-86.280816666666666</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="8"/>
       <c r="C55" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -1868,21 +1902,21 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row r="56" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B56" s="5">
         <v>100</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" s="6">
         <v>43.2</v>
       </c>
       <c r="E56" s="6">
-        <v>-86.51666666666667</v>
+        <v>-86.516666666666666</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>28</v>
@@ -1897,7 +1931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1905,22 +1939,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +1981,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1969,9 +1999,11 @@
       </c>
       <c r="F2" s="6">
         <f>B2+C2/60</f>
+        <v>43.2</v>
       </c>
       <c r="G2" s="6">
         <f>-(D2+E2/60)</f>
+        <v>-86.377833333333328</v>
       </c>
       <c r="H2" s="5">
         <v>25</v>
@@ -1980,7 +2012,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1998,9 +2030,11 @@
       </c>
       <c r="F3" s="6">
         <f>B3+C3/60</f>
+        <v>43.2</v>
       </c>
       <c r="G3" s="6">
         <f>-(D3+E3/60)</f>
+        <v>-86.516666666666666</v>
       </c>
       <c r="H3" s="5">
         <v>100</v>
@@ -2009,7 +2043,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
@@ -2017,26 +2051,28 @@
         <v>43</v>
       </c>
       <c r="C4" s="6">
-        <v>11.864</v>
+        <v>11.864000000000001</v>
       </c>
       <c r="D4" s="5">
         <v>86</v>
       </c>
       <c r="E4" s="6">
-        <v>58.335</v>
+        <v>58.335000000000001</v>
       </c>
       <c r="F4" s="6">
         <f>B4+C4/60</f>
+        <v>43.197733333333332</v>
       </c>
       <c r="G4" s="6">
         <f>-(D4+E4/60)</f>
+        <v>-86.972250000000003</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -2049,7 +2085,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -2057,19 +2093,21 @@
         <v>43</v>
       </c>
       <c r="C6" s="10">
-        <v>7.052</v>
+        <v>7.0519999999999996</v>
       </c>
       <c r="D6" s="5">
         <v>86</v>
       </c>
       <c r="E6" s="10">
-        <v>34.63</v>
+        <v>34.630000000000003</v>
       </c>
       <c r="F6" s="6">
         <f>B6+C6/60</f>
+        <v>43.117533333333334</v>
       </c>
       <c r="G6" s="6">
         <f>-(D6+E6/60)</f>
+        <v>-86.57716666666667</v>
       </c>
       <c r="H6" s="5">
         <v>103</v>
@@ -2080,7 +2118,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2088,7 +2126,7 @@
         <v>43</v>
       </c>
       <c r="C7" s="10">
-        <v>3.588</v>
+        <v>3.5880000000000001</v>
       </c>
       <c r="D7" s="5">
         <v>86</v>
@@ -2098,9 +2136,11 @@
       </c>
       <c r="F7" s="6">
         <f>B7+C7/60</f>
+        <v>43.059800000000003</v>
       </c>
       <c r="G7" s="6">
         <f>-(D7+E7/60)</f>
+        <v>-86.648333333333326</v>
       </c>
       <c r="H7" s="5">
         <v>102</v>
@@ -2111,7 +2151,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -2129,9 +2169,11 @@
       </c>
       <c r="F8" s="6">
         <f>B8+C8/60</f>
+        <v>43.225999999999999</v>
       </c>
       <c r="G8" s="6">
         <f>-(D8+E8/60)</f>
+        <v>-86.296333333333337</v>
       </c>
       <c r="H8" s="5">
         <v>22</v>
@@ -2144,7 +2186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -2162,9 +2204,11 @@
       </c>
       <c r="F9" s="6">
         <f>B9+C9/60</f>
+        <v>43.222166666666666</v>
       </c>
       <c r="G9" s="6">
         <f>-(D9+E9/60)</f>
+        <v>-86.280816666666666</v>
       </c>
       <c r="H9" s="5">
         <v>12</v>

</xml_diff>